<commit_message>
Create new footer [issue 53]
</commit_message>
<xml_diff>
--- a/retail_stores.xlsx
+++ b/retail_stores.xlsx
@@ -431,35 +431,35 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Shaw%27s General Store</v>
+        <v>American Eagle Store</v>
       </c>
       <c r="B3" t="str">
-        <v>44.465189</v>
+        <v>44.4648997</v>
       </c>
       <c r="C3" t="str">
-        <v>-72.686386</v>
+        <v>-73.1845057</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Urban Outfitters</v>
+        <v>T.J. Maxx</v>
       </c>
       <c r="B4" t="str">
-        <v>44.4798052</v>
+        <v>44.2242076</v>
       </c>
       <c r="C4" t="str">
-        <v>-73.213015</v>
+        <v>-72.5472328</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Catamount Store</v>
+        <v>Shaw%27s General Store</v>
       </c>
       <c r="B5" t="str">
-        <v>44.47899</v>
+        <v>44.465189</v>
       </c>
       <c r="C5" t="str">
-        <v>-73.212384</v>
+        <v>-72.686386</v>
       </c>
     </row>
     <row r="6">
@@ -475,13 +475,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>rue21</v>
+        <v>Sierra</v>
       </c>
       <c r="B7" t="str">
-        <v>44.4662295</v>
+        <v>44.4494116</v>
       </c>
       <c r="C7" t="str">
-        <v>-73.1833943</v>
+        <v>-73.2104912</v>
       </c>
     </row>
     <row r="8">
@@ -497,695 +497,695 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Miller%27s Country Store</v>
+        <v>rue21</v>
       </c>
       <c r="B9" t="str">
-        <v>44.5394208</v>
+        <v>44.4662295</v>
       </c>
       <c r="C9" t="str">
-        <v>-72.6166999</v>
+        <v>-73.1833943</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Sierra</v>
+        <v>Catamount Store</v>
       </c>
       <c r="B10" t="str">
-        <v>44.4494116</v>
+        <v>44.47899</v>
       </c>
       <c r="C10" t="str">
-        <v>-73.2104912</v>
+        <v>-73.212384</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>T.J. Maxx</v>
+        <v>Vermont Maple Outlet</v>
       </c>
       <c r="B11" t="str">
-        <v>44.2242076</v>
+        <v>44.6457139</v>
       </c>
       <c r="C11" t="str">
-        <v>-72.5472328</v>
+        <v>-72.8510611</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>The Country Store on Main</v>
+        <v>Orvis Outlet</v>
       </c>
       <c r="B12" t="str">
-        <v>44.4655025</v>
+        <v>43.171326</v>
       </c>
       <c r="C12" t="str">
-        <v>-72.6851814</v>
+        <v>-73.062804</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Lovermont 802</v>
+        <v>Vermont Discount Store</v>
       </c>
       <c r="B13" t="str">
-        <v>44.4652572</v>
+        <v>44.4580271</v>
       </c>
       <c r="C13" t="str">
-        <v>-73.1840663</v>
+        <v>-73.1277101</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>JCPenney</v>
+        <v>Urban Outfitters</v>
       </c>
       <c r="B14" t="str">
-        <v>44.4649765</v>
+        <v>44.4798052</v>
       </c>
       <c r="C14" t="str">
-        <v>-73.184073</v>
+        <v>-73.213015</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Whim Boutique</v>
+        <v>Theory Manchester Outlet</v>
       </c>
       <c r="B15" t="str">
-        <v>44.4785874</v>
+        <v>43.1759713</v>
       </c>
       <c r="C15" t="str">
-        <v>-73.2124573</v>
+        <v>-73.0558468</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Vermont Discount Store</v>
+        <v>Kohl%27s</v>
       </c>
       <c r="B16" t="str">
-        <v>44.4580271</v>
+        <v>44.4634379</v>
       </c>
       <c r="C16" t="str">
-        <v>-73.1277101</v>
+        <v>-73.1840006</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Shelburne Country Store</v>
+        <v>JCPenney</v>
       </c>
       <c r="B17" t="str">
-        <v>44.380394</v>
+        <v>44.4649765</v>
       </c>
       <c r="C17" t="str">
-        <v>-73.227066</v>
+        <v>-73.184073</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Church Street</v>
+        <v>Shelburne Country Store</v>
       </c>
       <c r="B18" t="str">
-        <v>44.4767527</v>
+        <v>44.380394</v>
       </c>
       <c r="C18" t="str">
-        <v>-73.2126288</v>
+        <v>-73.227066</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Orvis Outlet</v>
+        <v>The Vermont Country Store Weston</v>
       </c>
       <c r="B19" t="str">
-        <v>43.171326</v>
+        <v>43.2907845</v>
       </c>
       <c r="C19" t="str">
-        <v>-73.062804</v>
+        <v>-72.7927095</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Green Mountain Shopping Plaza Shopping Center</v>
+        <v>The Country Store on Main</v>
       </c>
       <c r="B20" t="str">
-        <v>43.5856463</v>
+        <v>44.4655025</v>
       </c>
       <c r="C20" t="str">
-        <v>-72.9699283</v>
+        <v>-72.6851814</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>The Vermont Country Store Weston</v>
+        <v>Free People</v>
       </c>
       <c r="B21" t="str">
-        <v>43.2907845</v>
+        <v>44.477898</v>
       </c>
       <c r="C21" t="str">
-        <v>-72.7927095</v>
+        <v>-73.212351</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Marimekko Outlet</v>
+        <v>The Country Store on Main</v>
       </c>
       <c r="B22" t="str">
-        <v>43.1752098</v>
+        <v>44.4655025</v>
       </c>
       <c r="C22" t="str">
-        <v>-73.0583729</v>
+        <v>-72.6851814</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>T.J. Maxx</v>
+        <v>Free People</v>
       </c>
       <c r="B23" t="str">
-        <v>44.2242076</v>
+        <v>44.477898</v>
       </c>
       <c r="C23" t="str">
-        <v>-72.5472328</v>
+        <v>-73.212351</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Kohl%27s</v>
+        <v>Marshalls</v>
       </c>
       <c r="B24" t="str">
-        <v>44.4634379</v>
+        <v>44.5733103</v>
       </c>
       <c r="C24" t="str">
-        <v>-73.1840006</v>
+        <v>-72.5918218</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Manchester Designer Outlets</v>
+        <v>Green Mountain Shopping Plaza Shopping Center</v>
       </c>
       <c r="B25" t="str">
-        <v>43.1759902</v>
+        <v>43.5856463</v>
       </c>
       <c r="C25" t="str">
-        <v>-73.0558157</v>
+        <v>-72.9699283</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Green Mountain Mall</v>
+        <v>Whim Boutique</v>
       </c>
       <c r="B26" t="str">
-        <v>44.4605822</v>
+        <v>44.4785874</v>
       </c>
       <c r="C26" t="str">
-        <v>-72.0135915</v>
+        <v>-73.2124573</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Lovermont 802</v>
+        <v>H%26M</v>
       </c>
       <c r="B27" t="str">
-        <v>44.4652572</v>
+        <v>44.4658817</v>
       </c>
       <c r="C27" t="str">
-        <v>-73.1840663</v>
+        <v>-73.184102</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Whim Boutique</v>
+        <v>Common Deer</v>
       </c>
       <c r="B28" t="str">
-        <v>44.4785874</v>
+        <v>44.4772305</v>
       </c>
       <c r="C28" t="str">
-        <v>-73.2124573</v>
+        <v>-73.2112009</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Fj%C3%A4llr%C3%A4ven Brand Store</v>
+        <v>Torrid</v>
       </c>
       <c r="B29" t="str">
-        <v>44.478972</v>
+        <v>44.445545</v>
       </c>
       <c r="C29" t="str">
-        <v>-73.2125441</v>
+        <v>-73.1099842</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>L.L.Bean</v>
+        <v>Vermont Gift Barn</v>
       </c>
       <c r="B30" t="str">
-        <v>44.44862</v>
+        <v>44.4685815</v>
       </c>
       <c r="C30" t="str">
-        <v>-73.1075015</v>
+        <v>-73.1802468</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Green Mountain Shopping Plaza Shopping Center</v>
+        <v>Fj%C3%A4llr%C3%A4ven Brand Store</v>
       </c>
       <c r="B31" t="str">
-        <v>43.5856463</v>
+        <v>44.478972</v>
       </c>
       <c r="C31" t="str">
-        <v>-72.9699283</v>
+        <v>-73.2125441</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Miller%27s Country Store</v>
+        <v>DICK%27S Sporting Goods</v>
       </c>
       <c r="B32" t="str">
-        <v>44.5394208</v>
+        <v>43.5850627</v>
       </c>
       <c r="C32" t="str">
-        <v>-72.6166999</v>
+        <v>-72.9708774</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Catamount Store</v>
+        <v>Harbour Thread, Clothes %26 Shoes for Women and Men</v>
       </c>
       <c r="B33" t="str">
-        <v>44.47899</v>
+        <v>44.4778323</v>
       </c>
       <c r="C33" t="str">
-        <v>-73.212384</v>
+        <v>-73.212352</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Essex Junction Shopping Center</v>
+        <v>Polo Ralph Lauren Factory Store</v>
       </c>
       <c r="B34" t="str">
-        <v>44.4949332</v>
+        <v>43.175947</v>
       </c>
       <c r="C34" t="str">
-        <v>-73.1202882</v>
+        <v>-73.0569779</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Outdoor Gear Exchange</v>
+        <v>Farm-Way Inc %2F Vermont Gear</v>
       </c>
       <c r="B35" t="str">
-        <v>44.4790418</v>
+        <v>43.9810278</v>
       </c>
       <c r="C35" t="str">
-        <v>-73.2132079</v>
+        <v>-72.1166221</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>The Vermont Country Store Rockingham</v>
+        <v>Marimekko Outlet</v>
       </c>
       <c r="B36" t="str">
-        <v>43.1973556</v>
+        <v>43.1752098</v>
       </c>
       <c r="C36" t="str">
-        <v>-72.505125</v>
+        <v>-73.0583729</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Patagonia Burlington</v>
+        <v>Banana Republic</v>
       </c>
       <c r="B37" t="str">
-        <v>44.4770013</v>
+        <v>44.4787285</v>
       </c>
       <c r="C37" t="str">
-        <v>-73.2119478</v>
+        <v>-73.2123065</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>REI</v>
+        <v>T.J. Maxx</v>
       </c>
       <c r="B38" t="str">
-        <v>44.4434577</v>
+        <v>44.0014199</v>
       </c>
       <c r="C38" t="str">
-        <v>-73.1141099</v>
+        <v>-73.1555297</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Theory Manchester Outlet</v>
+        <v>Old Navy</v>
       </c>
       <c r="B39" t="str">
-        <v>43.1759713</v>
+        <v>44.442698</v>
       </c>
       <c r="C39" t="str">
-        <v>-73.0558468</v>
+        <v>-73.1105473</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Torrid</v>
+        <v>Outdoor Gear Exchange</v>
       </c>
       <c r="B40" t="str">
-        <v>44.445545</v>
+        <v>44.4790418</v>
       </c>
       <c r="C40" t="str">
-        <v>-73.1099842</v>
+        <v>-73.2132079</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Harbour Thread, Clothes %26 Shoes for Women and Men</v>
+        <v>Vermont Eclectic Company</v>
       </c>
       <c r="B41" t="str">
-        <v>44.4778323</v>
+        <v>43.6253986</v>
       </c>
       <c r="C41" t="str">
-        <v>-73.212352</v>
+        <v>-72.517986</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>DICK%27S Sporting Goods</v>
+        <v>The Vermont Flannel Co.</v>
       </c>
       <c r="B42" t="str">
-        <v>44.4428517</v>
+        <v>44.479655</v>
       </c>
       <c r="C42" t="str">
-        <v>-73.1111562</v>
+        <v>-73.2125771</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Alpine Shop VT</v>
+        <v>Lovermont 802</v>
       </c>
       <c r="B43" t="str">
-        <v>44.4441086</v>
+        <v>44.4787346</v>
       </c>
       <c r="C43" t="str">
-        <v>-73.2123616</v>
+        <v>-73.2128758</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Free People</v>
+        <v>Jess Boutique</v>
       </c>
       <c r="B44" t="str">
-        <v>44.477898</v>
+        <v>44.477734</v>
       </c>
       <c r="C44" t="str">
-        <v>-73.212351</v>
+        <v>-73.212334</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Old Navy</v>
+        <v>DICK%27S Sporting Goods</v>
       </c>
       <c r="B45" t="str">
-        <v>44.442698</v>
+        <v>44.4428517</v>
       </c>
       <c r="C45" t="str">
-        <v>-73.1105473</v>
+        <v>-73.1111562</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>DICK%27S Sporting Goods</v>
+        <v>H N Williams Store</v>
       </c>
       <c r="B46" t="str">
-        <v>43.5850627</v>
+        <v>43.247203</v>
       </c>
       <c r="C46" t="str">
-        <v>-72.9708774</v>
+        <v>-73.091897</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Ten Thousand Villages</v>
+        <v>HomeGoods</v>
       </c>
       <c r="B47" t="str">
-        <v>44.477885</v>
+        <v>44.4497578</v>
       </c>
       <c r="C47" t="str">
-        <v>-73.212826</v>
+        <v>-73.2108346</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Marshalls</v>
+        <v>University Mall</v>
       </c>
       <c r="B48" t="str">
-        <v>44.5733103</v>
+        <v>44.4658817</v>
       </c>
       <c r="C48" t="str">
-        <v>-72.5918218</v>
+        <v>-73.184102</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Vermont Eclectic Company</v>
+        <v>Coco Goose Burlington</v>
       </c>
       <c r="B49" t="str">
-        <v>43.6253986</v>
+        <v>44.4753962</v>
       </c>
       <c r="C49" t="str">
-        <v>-72.517986</v>
+        <v>-73.2188707</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Polo Ralph Lauren Factory Store</v>
+        <v>Lovermont 802</v>
       </c>
       <c r="B50" t="str">
-        <v>43.175947</v>
+        <v>44.4652572</v>
       </c>
       <c r="C50" t="str">
-        <v>-73.0569779</v>
+        <v>-73.1840663</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Goodwill Retail Store</v>
+        <v>Ten Thousand Villages</v>
       </c>
       <c r="B51" t="str">
-        <v>43.6246011</v>
+        <v>44.477885</v>
       </c>
       <c r="C51" t="str">
-        <v>-72.9747188</v>
+        <v>-73.212826</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Replays</v>
+        <v>Church Street</v>
       </c>
       <c r="B52" t="str">
-        <v>44.4651686</v>
+        <v>44.4767527</v>
       </c>
       <c r="C52" t="str">
-        <v>-73.1793338</v>
+        <v>-73.2126288</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Golden Hour Gift Co %28formerly Trinket%29</v>
+        <v>Old Gold</v>
       </c>
       <c r="B53" t="str">
-        <v>44.4795062</v>
+        <v>44.479198</v>
       </c>
       <c r="C53" t="str">
-        <v>-73.212561</v>
+        <v>-73.2119781</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Walmart</v>
+        <v>Gateway Shopping Center</v>
       </c>
       <c r="B54" t="str">
-        <v>44.4415818</v>
+        <v>44.4496407</v>
       </c>
       <c r="C54" t="str">
-        <v>-73.1222042</v>
+        <v>-73.2077537</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>North Avenue Shopping Center</v>
+        <v>Orvis</v>
       </c>
       <c r="B55" t="str">
-        <v>44.5081977</v>
+        <v>43.1690067</v>
       </c>
       <c r="C55" t="str">
-        <v>-73.2473373</v>
+        <v>-73.0657506</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>The Vermont Flannel Co.</v>
+        <v>The Vermont Country Store Rockingham</v>
       </c>
       <c r="B56" t="str">
-        <v>44.479655</v>
+        <v>43.1973556</v>
       </c>
       <c r="C56" t="str">
-        <v>-73.2125771</v>
+        <v>-72.505125</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Lovermont 802</v>
+        <v>Vermont Marketplace</v>
       </c>
       <c r="B57" t="str">
-        <v>44.4787346</v>
+        <v>42.8360545</v>
       </c>
       <c r="C57" t="str">
-        <v>-73.2128758</v>
+        <v>-72.5659773</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Orvis</v>
+        <v>Golden Hour Gift Co %28formerly Trinket%29</v>
       </c>
       <c r="B58" t="str">
-        <v>43.1690067</v>
+        <v>44.4795062</v>
       </c>
       <c r="C58" t="str">
-        <v>-73.0657506</v>
+        <v>-73.212561</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Vintage Inspired Marketplace</v>
+        <v>Keep Vermont Weird</v>
       </c>
       <c r="B59" t="str">
-        <v>44.468327</v>
+        <v>44.479551</v>
       </c>
       <c r="C59" t="str">
-        <v>-73.1809997</v>
+        <v>-73.2128999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>SavvyShoppingClub</v>
+        <v>REI</v>
       </c>
       <c r="B60" t="str">
-        <v>44.4784225</v>
+        <v>44.4434577</v>
       </c>
       <c r="C60" t="str">
-        <v>-73.2106541</v>
+        <v>-73.1141099</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Essex Experience</v>
+        <v>The Vermont Spot</v>
       </c>
       <c r="B61" t="str">
-        <v>44.5069978</v>
+        <v>43.6380054</v>
       </c>
       <c r="C61" t="str">
-        <v>-73.0820468</v>
+        <v>-72.3979446</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>HomeGoods</v>
+        <v>The Vermont Flannel Co.</v>
       </c>
       <c r="B62" t="str">
-        <v>44.4497578</v>
+        <v>44.159916</v>
       </c>
       <c r="C62" t="str">
-        <v>-73.2108346</v>
+        <v>-72.4510307</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Best Buy</v>
+        <v>Quechee Gorge Village</v>
       </c>
       <c r="B63" t="str">
-        <v>44.444704</v>
+        <v>43.638063</v>
       </c>
       <c r="C63" t="str">
-        <v>-73.109586</v>
+        <v>-72.397759</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Vermont%27s Own Gifts %26 Goods</v>
+        <v>Walmart</v>
       </c>
       <c r="B64" t="str">
-        <v>44.0131272</v>
+        <v>44.4415818</v>
       </c>
       <c r="C64" t="str">
-        <v>-73.1690017</v>
+        <v>-73.1222042</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>The Vermont Spot</v>
+        <v>Alpine Shop</v>
       </c>
       <c r="B65" t="str">
-        <v>43.6380054</v>
+        <v>44.4441086</v>
       </c>
       <c r="C65" t="str">
-        <v>-72.3979446</v>
+        <v>-73.2123616</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>H N Williams Store</v>
+        <v>SavvyShoppingClub</v>
       </c>
       <c r="B66" t="str">
-        <v>43.247203</v>
+        <v>44.4784225</v>
       </c>
       <c r="C66" t="str">
-        <v>-73.091897</v>
+        <v>-73.2106541</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Vermont Flannel Factory Store</v>
+        <v>Billie Jean Vintage</v>
       </c>
       <c r="B67" t="str">
-        <v>44.6103594</v>
+        <v>44.4753821</v>
       </c>
       <c r="C67" t="str">
-        <v>-72.6489825</v>
+        <v>-73.218397</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Banana Republic</v>
+        <v>Replays</v>
       </c>
       <c r="B68" t="str">
-        <v>44.4787285</v>
+        <v>44.4651686</v>
       </c>
       <c r="C68" t="str">
-        <v>-73.2123065</v>
+        <v>-73.1793338</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>H%26M</v>
+        <v>Goodwill Retail Store</v>
       </c>
       <c r="B69" t="str">
-        <v>44.4658817</v>
+        <v>43.6246011</v>
       </c>
       <c r="C69" t="str">
-        <v>-73.184102</v>
+        <v>-72.9747188</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Rutland Plaza - Rutland</v>
+        <v>Bargain Boutique</v>
       </c>
       <c r="B70" t="str">
-        <v>43.6061923</v>
+        <v>44.3370481</v>
       </c>
       <c r="C70" t="str">
-        <v>-72.9793973</v>
+        <v>-72.7554347</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Above All Vermont</v>
+        <v>Green Mountain Mall</v>
       </c>
       <c r="B71" t="str">
-        <v>43.1747643</v>
+        <v>44.4605822</v>
       </c>
       <c r="C71" t="str">
-        <v>-73.0537255</v>
+        <v>-72.0135915</v>
       </c>
     </row>
     <row r="72">
@@ -1201,321 +1201,321 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Shelburne Road Shopping Plaza</v>
+        <v>Vintage Inspired Marketplace</v>
       </c>
       <c r="B73" t="str">
-        <v>44.4497327</v>
+        <v>44.468327</v>
       </c>
       <c r="C73" t="str">
-        <v>-73.2098014</v>
+        <v>-73.1809997</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Vermont Antique Mall</v>
+        <v>Style Encore Williston</v>
       </c>
       <c r="B74" t="str">
-        <v>43.6379689</v>
+        <v>44.4506504</v>
       </c>
       <c r="C74" t="str">
-        <v>-72.3974961</v>
+        <v>-73.1093768</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>The Vermont Flannel Co.</v>
+        <v>Apple Island General Store</v>
       </c>
       <c r="B75" t="str">
-        <v>43.6255216</v>
+        <v>44.635658</v>
       </c>
       <c r="C75" t="str">
-        <v>-72.5183327</v>
+        <v>-73.2667619</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Original Vermont Store</v>
+        <v>lululemon</v>
       </c>
       <c r="B76" t="str">
-        <v>43.516876</v>
+        <v>44.4795577</v>
       </c>
       <c r="C76" t="str">
-        <v>-73.236137</v>
+        <v>-73.2132069</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Vermont Flannel Factory Store</v>
+        <v>Vermont Outfitters Co</v>
       </c>
       <c r="B77" t="str">
-        <v>44.159916</v>
+        <v>43.044766</v>
       </c>
       <c r="C77" t="str">
-        <v>-72.4510307</v>
+        <v>-72.923805</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>lululemon</v>
+        <v>Manchester Designer Outlets</v>
       </c>
       <c r="B78" t="str">
-        <v>44.4795577</v>
+        <v>43.1759902</v>
       </c>
       <c r="C78" t="str">
-        <v>-73.2132069</v>
+        <v>-73.0558157</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>Bargain Boutique</v>
+        <v>The Vermont Flannel Co.</v>
       </c>
       <c r="B79" t="str">
-        <v>44.3370481</v>
+        <v>44.6103594</v>
       </c>
       <c r="C79" t="str">
-        <v>-72.7554347</v>
+        <v>-72.6489825</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>The Vermont Flannel Co.</v>
+        <v>Above All Vermont</v>
       </c>
       <c r="B80" t="str">
-        <v>44.237737</v>
+        <v>43.1747643</v>
       </c>
       <c r="C80" t="str">
-        <v>-73.2319604</v>
+        <v>-73.0537255</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Village Court Shopping Center</v>
+        <v>Pendleton</v>
       </c>
       <c r="B81" t="str">
-        <v>44.0107271</v>
+        <v>43.1733305</v>
       </c>
       <c r="C81" t="str">
-        <v>-73.1645384</v>
+        <v>-73.0499471</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Taft Corners Shopping Center</v>
+        <v>What to Wear Boutique</v>
       </c>
       <c r="B82" t="str">
-        <v>44.4506055</v>
+        <v>44.418884</v>
       </c>
       <c r="C82" t="str">
-        <v>-73.1098173</v>
+        <v>-72.015374</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>100 Dorset</v>
+        <v>The Vermont Flannel Company</v>
       </c>
       <c r="B83" t="str">
-        <v>44.4671064</v>
+        <v>44.237737</v>
       </c>
       <c r="C83" t="str">
-        <v>-73.1803473</v>
+        <v>-73.2319604</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>J.Crew Factory</v>
+        <v>Vermont%27s Own Gifts %26 Goods</v>
       </c>
       <c r="B84" t="str">
-        <v>43.1744874</v>
+        <v>44.0131272</v>
       </c>
       <c r="C84" t="str">
-        <v>-73.0513647</v>
+        <v>-73.1690017</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>Goodwill Store: South Burlington</v>
+        <v>Burton Burlington Headquarters Flagship Store</v>
       </c>
       <c r="B85" t="str">
-        <v>44.4391634</v>
+        <v>44.4488409</v>
       </c>
       <c r="C85" t="str">
-        <v>-73.2096079</v>
+        <v>-73.219772</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>Underground Closet</v>
+        <v>Gift Shop</v>
       </c>
       <c r="B86" t="str">
-        <v>44.4798446</v>
+        <v>44.4689589</v>
       </c>
       <c r="C86" t="str">
-        <v>-73.2129366</v>
+        <v>-73.1550272</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Northeast Kingdom Country Store</v>
+        <v>The Collection</v>
       </c>
       <c r="B87" t="str">
-        <v>44.5880165</v>
+        <v>44.184354</v>
       </c>
       <c r="C87" t="str">
-        <v>-71.9448013</v>
+        <v>-72.839175</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>Vermont Discount Store</v>
+        <v>Vermont Clothes</v>
       </c>
       <c r="B88" t="str">
-        <v>43.6128509</v>
+        <v>44.8362873</v>
       </c>
       <c r="C88" t="str">
-        <v>-72.9884187</v>
+        <v>-73.0994782</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>Style Encore Williston</v>
+        <v>April Cornell</v>
       </c>
       <c r="B89" t="str">
-        <v>44.4506504</v>
+        <v>44.47608</v>
       </c>
       <c r="C89" t="str">
-        <v>-73.1093768</v>
+        <v>-73.2190472</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Pendleton</v>
+        <v>Vermont Discount Store</v>
       </c>
       <c r="B90" t="str">
-        <v>43.1733305</v>
+        <v>43.6128509</v>
       </c>
       <c r="C90" t="str">
-        <v>-73.0499471</v>
+        <v>-72.9884187</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Dorset Union Store</v>
+        <v>Homeport</v>
       </c>
       <c r="B91" t="str">
-        <v>43.2544878</v>
+        <v>44.478863</v>
       </c>
       <c r="C91" t="str">
-        <v>-73.0992575</v>
+        <v>-73.212327</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>The Collection</v>
+        <v>Maple Tree Place</v>
       </c>
       <c r="B92" t="str">
-        <v>44.184354</v>
+        <v>44.4451629</v>
       </c>
       <c r="C92" t="str">
-        <v>-72.839175</v>
+        <v>-73.1093402</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>What to Wear Boutique</v>
+        <v>North Avenue Shopping Center</v>
       </c>
       <c r="B93" t="str">
-        <v>44.418884</v>
+        <v>44.5081977</v>
       </c>
       <c r="C93" t="str">
-        <v>-72.015374</v>
+        <v>-73.2473373</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>The Vermont Flannel Co.</v>
+        <v>Sensible Shoe</v>
       </c>
       <c r="B94" t="str">
-        <v>43.1753883</v>
+        <v>43.6226281</v>
       </c>
       <c r="C94" t="str">
-        <v>-73.0556082</v>
+        <v>-72.9533903</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>The Vermont Book Shop</v>
+        <v>First Chair Retail</v>
       </c>
       <c r="B95" t="str">
-        <v>44.013969</v>
+        <v>44.5302518</v>
       </c>
       <c r="C95" t="str">
-        <v>-73.168541</v>
+        <v>-72.7807646</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Walmart</v>
+        <v>Underground Closet</v>
       </c>
       <c r="B96" t="str">
-        <v>43.6053053</v>
+        <v>44.4798446</v>
       </c>
       <c r="C96" t="str">
-        <v>-72.980631</v>
+        <v>-73.2129366</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>Central Vermont Marketplace</v>
+        <v>Johnson Woolen Mills</v>
       </c>
       <c r="B97" t="str">
-        <v>44.2169004</v>
+        <v>44.6350024</v>
       </c>
       <c r="C97" t="str">
-        <v>-72.5646455</v>
+        <v>-72.6782002</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>Entrep%C3%B4t Costco</v>
+        <v>Goodwill Store: South Burlington</v>
       </c>
       <c r="B98" t="str">
-        <v>44.5039486</v>
+        <v>44.4391634</v>
       </c>
       <c r="C98" t="str">
-        <v>-73.1743212</v>
+        <v>-73.2096079</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Willey%27s Store Inc.</v>
+        <v>Original Vermont Store</v>
       </c>
       <c r="B99" t="str">
-        <v>44.5757324</v>
+        <v>43.516876</v>
       </c>
       <c r="C99" t="str">
-        <v>-72.2955416</v>
+        <v>-73.236137</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Weston Village Store</v>
+        <v>Vermont Gift %26 Garden Center</v>
       </c>
       <c r="B100" t="str">
-        <v>43.2909183</v>
+        <v>43.6516771</v>
       </c>
       <c r="C100" t="str">
-        <v>-72.7931857</v>
+        <v>-72.8927094</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>Shelburne Square</v>
+        <v>Lenny%27s Shoe %26 Apparel</v>
       </c>
       <c r="B101" t="str">
-        <v>44.4337637</v>
+        <v>44.451779</v>
       </c>
       <c r="C101" t="str">
-        <v>-73.2098598</v>
+        <v>-73.1110283</v>
       </c>
     </row>
     <row r="102">
@@ -1531,178 +1531,178 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>Vermont Marketplace</v>
+        <v>100 Dorset</v>
       </c>
       <c r="B103" t="str">
-        <v>44.1328741</v>
+        <v>44.4671064</v>
       </c>
       <c r="C103" t="str">
-        <v>-73.0775669</v>
+        <v>-73.1803473</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>Vermont Gift Barn</v>
+        <v>Taft Corners Shopping Center</v>
       </c>
       <c r="B104" t="str">
-        <v>44.4685815</v>
+        <v>44.4506055</v>
       </c>
       <c r="C104" t="str">
-        <v>-73.1802468</v>
+        <v>-73.1098173</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Common Deer</v>
+        <v>Vermont Food and Gifts-New World Enterprises, Inc.</v>
       </c>
       <c r="B105" t="str">
-        <v>44.4772305</v>
+        <v>44.4988257</v>
       </c>
       <c r="C105" t="str">
-        <v>-73.2112009</v>
+        <v>-73.183825</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>Gift Shop</v>
+        <v>Weston Village Store</v>
       </c>
       <c r="B106" t="str">
-        <v>44.4689589</v>
+        <v>43.2909183</v>
       </c>
       <c r="C106" t="str">
-        <v>-73.1550272</v>
+        <v>-72.7931857</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Onion River Outdoors</v>
+        <v>Best Buy</v>
       </c>
       <c r="B107" t="str">
-        <v>44.2602388</v>
+        <v>44.444704</v>
       </c>
       <c r="C107" t="str">
-        <v>-72.5746165</v>
+        <v>-73.109586</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Barnard General Store</v>
+        <v>Shelburne Road Shopping Plaza</v>
       </c>
       <c r="B108" t="str">
-        <v>43.728348</v>
+        <v>44.4497327</v>
       </c>
       <c r="C108" t="str">
-        <v>-72.6186387</v>
+        <v>-73.2098014</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Eastern Mountain Sports</v>
+        <v>Golden Hour Gift Co %28formerly Birdfolk Collective%29</v>
       </c>
       <c r="B109" t="str">
-        <v>44.4636557</v>
+        <v>44.4915321</v>
       </c>
       <c r="C109" t="str">
-        <v>-73.1797377</v>
+        <v>-73.1857919</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Burton Burlington Headquarters Flagship Store</v>
+        <v>Eastern Mountain Sports</v>
       </c>
       <c r="B110" t="str">
-        <v>44.4488409</v>
+        <v>44.4636557</v>
       </c>
       <c r="C110" t="str">
-        <v>-73.219772</v>
+        <v>-73.1797377</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Vermont Food and Gifts-New World Enterprises, Inc.</v>
+        <v>Vermont Gift Emporium</v>
       </c>
       <c r="B111" t="str">
-        <v>44.4988257</v>
+        <v>42.8360919</v>
       </c>
       <c r="C111" t="str">
-        <v>-73.183825</v>
+        <v>-72.5653089</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>First Chair Retail</v>
+        <v>Vermont Shopping Center</v>
       </c>
       <c r="B112" t="str">
-        <v>44.5302518</v>
+        <v>44.2292674</v>
       </c>
       <c r="C112" t="str">
-        <v>-72.7807646</v>
+        <v>-72.5516881</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>Sensible Shoe</v>
+        <v>Vermont Marketplace</v>
       </c>
       <c r="B113" t="str">
-        <v>43.6226281</v>
+        <v>44.1328741</v>
       </c>
       <c r="C113" t="str">
-        <v>-72.9533903</v>
+        <v>-73.0775669</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>Mammut Sports Group Inc</v>
+        <v>New England Via Vermont</v>
       </c>
       <c r="B114" t="str">
-        <v>44.436454</v>
+        <v>45.0065013</v>
       </c>
       <c r="C114" t="str">
-        <v>-73.1060848</v>
+        <v>-73.2935267</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>Vermont Shopping Center</v>
+        <v>Vermont Antique Mall</v>
       </c>
       <c r="B115" t="str">
-        <v>44.2292674</v>
+        <v>43.6379689</v>
       </c>
       <c r="C115" t="str">
-        <v>-72.5516881</v>
+        <v>-72.3974961</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>Spellbound Vermont</v>
+        <v>Saint Albans Shopping Center</v>
       </c>
       <c r="B116" t="str">
-        <v>44.4775</v>
+        <v>44.815165</v>
       </c>
       <c r="C116" t="str">
-        <v>-73.2124</v>
+        <v>-73.0818696</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>US Sherpa</v>
+        <v>The Home Shop</v>
       </c>
       <c r="B117" t="str">
-        <v>44.4961901</v>
+        <v>43.799505</v>
       </c>
       <c r="C117" t="str">
-        <v>-73.1852618</v>
+        <v>-73.088565</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>Battery Street Jeans Exchange</v>
+        <v>US Sherpa</v>
       </c>
       <c r="B118" t="str">
-        <v>44.476831</v>
+        <v>44.4961901</v>
       </c>
       <c r="C118" t="str">
-        <v>-73.215192</v>
+        <v>-73.1852618</v>
       </c>
     </row>
     <row r="119">
@@ -1718,24 +1718,24 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Lenny%27s Shoe %26 Apparel</v>
+        <v>Highgate Commons Shopping Center</v>
       </c>
       <c r="B120" t="str">
-        <v>44.451779</v>
+        <v>44.840477</v>
       </c>
       <c r="C120" t="str">
-        <v>-73.1110283</v>
+        <v>-73.0800891</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>The Shopping Bag</v>
+        <v>Barge Canal Market</v>
       </c>
       <c r="B121" t="str">
-        <v>44.484848</v>
+        <v>44.4688017</v>
       </c>
       <c r="C121" t="str">
-        <v>-73.2154209</v>
+        <v>-73.2158559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>